<commit_message>
Actualizacion final Proyecto Migrador v2.0.
</commit_message>
<xml_diff>
--- a/laboratorio/pentaho/migrador_csv_to_db/docs/etl_reporting_monitoreo.xlsx
+++ b/laboratorio/pentaho/migrador_csv_to_db/docs/etl_reporting_monitoreo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\FPUNA\cit_bigdata_basico\laboratorio\pentaho\migrador_csv_to_db\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\fpuna\cit_bigdata_basico\laboratorio\pentaho\migrador_csv_to_db\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC82B5D-BE35-44A5-B8D5-ED902DC3F177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FCBFD6-E4FC-459C-AAB4-E74A24C4AF08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{0445F218-DF09-4B75-B0A3-340DC2DE20F8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0445F218-DF09-4B75-B0A3-340DC2DE20F8}"/>
   </bookViews>
   <sheets>
     <sheet name="RAW" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
   <si>
     <t>VW_NIVEL</t>
   </si>
@@ -82,9 +82,6 @@
     <t>DATASET</t>
   </si>
   <si>
-    <t>CA NTIDAD</t>
-  </si>
-  <si>
     <t>tipo_discapacidad</t>
   </si>
   <si>
@@ -152,6 +149,33 @@
   </si>
   <si>
     <t>PARAMETRICA</t>
+  </si>
+  <si>
+    <t>funcionarios_2023_01</t>
+  </si>
+  <si>
+    <t>BRUTO</t>
+  </si>
+  <si>
+    <t>CRUDO</t>
+  </si>
+  <si>
+    <t>ELIMINADO</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>PY</t>
+  </si>
+  <si>
+    <t>EXT</t>
   </si>
 </sst>
 </file>
@@ -195,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -208,6 +232,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -543,30 +570,161 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0882604-64B7-487A-A324-ADDDFDCDC1CE}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="11.5546875" style="1"/>
+    <col min="3" max="7" width="11.5546875" style="1"/>
+    <col min="8" max="8" width="11.5546875" style="5"/>
+    <col min="9" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="B2" s="2">
-        <v>942184</v>
+        <v>862950</v>
+      </c>
+      <c r="C2" s="2">
+        <v>6825</v>
+      </c>
+      <c r="D2" s="2">
+        <f>B2-C2</f>
+        <v>856125</v>
+      </c>
+      <c r="H2" s="5">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2">
+        <v>148522</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H3" s="5">
+        <v>2</v>
+      </c>
+      <c r="I3" s="2">
+        <v>166164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H4" s="5">
+        <v>3</v>
+      </c>
+      <c r="I4" s="2">
+        <v>204020</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H5" s="5">
+        <v>4</v>
+      </c>
+      <c r="I5" s="2">
+        <v>120775</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H6" s="5">
+        <v>5</v>
+      </c>
+      <c r="I6" s="2">
+        <v>40029</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H7" s="5">
+        <v>6</v>
+      </c>
+      <c r="I7" s="2">
+        <v>17699</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H8" s="5">
+        <v>7</v>
+      </c>
+      <c r="I8" s="2">
+        <v>13442</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H9" s="5">
+        <v>8</v>
+      </c>
+      <c r="I9" s="2">
+        <v>14448</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H10" s="5">
+        <v>9</v>
+      </c>
+      <c r="I10" s="2">
+        <v>15684</v>
+      </c>
+      <c r="J10" s="2">
+        <f>+SUM(I2:I10)</f>
+        <v>740783</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="2">
+        <v>120</v>
+      </c>
+      <c r="J11" s="1">
+        <v>120</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" s="2">
+        <v>8498</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="2">
+        <v>106724</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J15" s="2">
+        <f>+SUM(I13:I14)</f>
+        <v>115222</v>
       </c>
     </row>
   </sheetData>
@@ -719,7 +877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2089D6F3-420B-4635-8FCB-DC0B7B929F6B}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
@@ -743,7 +901,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -751,13 +909,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2">
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -765,13 +923,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2">
         <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -779,13 +937,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2">
         <v>4</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -793,13 +951,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -807,13 +965,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2">
         <v>4</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -821,13 +979,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2">
         <v>168</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -835,13 +993,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="2">
         <v>16</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -849,13 +1007,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="2">
         <v>9</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -863,13 +1021,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="2">
         <v>67</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -877,13 +1035,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="2">
         <v>368</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -891,13 +1049,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="2">
         <v>14</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -905,13 +1063,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="2">
         <v>122</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -919,13 +1077,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="2">
         <v>401</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -933,13 +1091,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="2">
         <v>270997</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -947,13 +1105,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="2">
         <v>295141</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -961,13 +1119,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="2">
         <v>16352</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -975,13 +1133,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="2">
         <v>6107</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -989,13 +1147,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="2">
         <v>444139</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1003,13 +1161,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="2">
         <v>444139</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1017,13 +1175,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="2">
         <v>770640</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>